<commit_message>
updating component 2 spray drift analysis
</commit_message>
<xml_diff>
--- a/00_Data/Master_files/COMP2_spray_drift.xlsx
+++ b/00_Data/Master_files/COMP2_spray_drift.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabelsmith/Documents/00_UQ_offline/STJW_analysis/00_Data/Master_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BEA93D-FCFC-A340-927C-EC5C4A7B66EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A641FD0C-96C9-974C-A4A9-C53E48A4D823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" activeTab="1" xr2:uid="{27DA9487-7295-D647-9057-457C5E0E1BA3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="57">
   <si>
     <t>location</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>Spot</t>
+  </si>
+  <si>
+    <t>Fine</t>
+  </si>
+  <si>
+    <t>Coarse</t>
   </si>
 </sst>
 </file>
@@ -633,24 +645,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0DE6A8-A443-8A4E-A653-D36658B31562}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="3" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,156 +670,174 @@
         <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>325268</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>273327</v>
       </c>
-      <c r="G2" s="1">
-        <f>1-F2/E2</f>
+      <c r="H2" s="1">
+        <f>1-G2/F2</f>
         <v>0.1596867813618309</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="1">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>302032</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>254311</v>
       </c>
-      <c r="G3" s="1">
-        <f>1-F3/E3</f>
+      <c r="H3" s="1">
+        <f>1-G3/F3</f>
         <v>0.15799981458918255</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>348692</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>278840</v>
       </c>
-      <c r="G4" s="1">
-        <f>1-F4/E4</f>
+      <c r="H4" s="1">
+        <f>1-G4/F4</f>
         <v>0.20032578894841291</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>324470</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>282636</v>
       </c>
-      <c r="G5" s="1">
-        <f>1-F5/E5</f>
+      <c r="H5" s="1">
+        <f>1-G5/F5</f>
         <v>0.12893025549357418</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>318986</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>241534</v>
       </c>
-      <c r="G6" s="1">
-        <f>1-F6/E6</f>
+      <c r="H6" s="1">
+        <f>1-G6/F6</f>
         <v>0.2428068943464603</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>13</v>
@@ -815,578 +845,653 @@
       <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="1">
         <v>4</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>392946</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>8643</v>
       </c>
-      <c r="G8" s="1">
-        <f t="shared" ref="G8:G21" si="0">1-F8/E8</f>
+      <c r="H8" s="1">
+        <f t="shared" ref="H8:H21" si="0">1-G8/F8</f>
         <v>0.97800461132063943</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1">
         <v>3</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>398426</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>2679</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <f t="shared" si="0"/>
         <v>0.99327604122220936</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="1">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>396621</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>6068</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <f t="shared" si="0"/>
         <v>0.98470075966728943</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>402866</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>70534</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <f t="shared" si="0"/>
         <v>0.82491945212552065</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>415928</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>333691</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <f t="shared" si="0"/>
         <v>0.19771931680483157</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1">
         <v>4</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>416675</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>341194</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <f t="shared" si="0"/>
         <v>0.18115077698446036</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="1">
         <v>3</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>413141</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>338875</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <f t="shared" si="0"/>
         <v>0.17975945258398462</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="1">
         <v>2</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>419993</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>324679</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <f t="shared" si="0"/>
         <v>0.226941877602722</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>423744</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>321349</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <f t="shared" si="0"/>
         <v>0.24164353949554451</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="1">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>341181</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>326707</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <f t="shared" si="0"/>
         <v>4.242322989849967E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1">
         <v>4</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>368330</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>289185</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <f t="shared" si="0"/>
         <v>0.2148752477397986</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="1">
         <v>3</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>365756</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>294199</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <f t="shared" si="0"/>
         <v>0.19564135653277048</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1">
         <v>2</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>362542</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>325409</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <f t="shared" si="0"/>
         <v>0.1024239950129916</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1">
         <v>2</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>375173</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>361397</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <f t="shared" si="0"/>
         <v>3.6719060273527115E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="1">
-        <v>5</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>363740</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>107343</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>0.70489085610600977</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1">
         <v>4</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>374680</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>16301</v>
       </c>
-      <c r="G23" s="1">
-        <f t="shared" ref="G23:G31" si="1">1-F23/E23</f>
+      <c r="H23" s="1">
+        <f t="shared" ref="H23:H31" si="1">1-G23/F23</f>
         <v>0.95649354115511909</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="1">
         <v>3</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>405444</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>1069</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <f t="shared" si="1"/>
         <v>0.99736338433914429</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="1">
         <v>2</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>448208</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>81354</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <f t="shared" si="1"/>
         <v>0.81849052225752328</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1">
         <v>1</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>402396</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>382</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <f t="shared" si="1"/>
         <v>0.99905068638853267</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="1">
-        <v>5</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="1">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>439616</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>369644</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <f t="shared" si="1"/>
         <v>0.15916618139467176</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="1">
         <v>4</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>458072</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>427963</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <f t="shared" si="1"/>
         <v>6.5729841596954164E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="1">
         <v>3</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>470438</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>402797</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <f t="shared" si="1"/>
         <v>0.14378302773160334</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="1">
         <v>2</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>484027</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>436267</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <f t="shared" si="1"/>
         <v>9.8672181510535584E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="1">
         <v>1</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>485797</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>408312</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <f t="shared" si="1"/>
         <v>0.15950077913202432</v>
       </c>

</xml_diff>